<commit_message>
working working i think
</commit_message>
<xml_diff>
--- a/blank_processed.xlsx
+++ b/blank_processed.xlsx
@@ -1151,7 +1151,7 @@
     <outlinePr summaryBelow="0" summaryRight="0"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AX1003"/>
+  <dimension ref="A1:AX1001"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
       <pane xSplit="13" topLeftCell="N1" activePane="topRight" state="frozen"/>
@@ -1491,15 +1491,15 @@
       <c r="P3" s="33" t="n"/>
       <c r="Q3" s="33" t="n"/>
       <c r="R3" s="35" t="n"/>
-      <c r="S3" s="36" t="n"/>
-      <c r="T3" s="36" t="n"/>
+      <c r="S3" s="36" t="n">
+        <v>31.45</v>
+      </c>
+      <c r="T3" s="36" t="inlineStr"/>
       <c r="U3" s="37" t="n">
         <v>20</v>
       </c>
-      <c r="V3" s="38" t="n">
-        <v>31.45</v>
-      </c>
-      <c r="W3" s="38" t="inlineStr"/>
+      <c r="V3" s="38" t="n"/>
+      <c r="W3" s="38" t="n"/>
       <c r="X3" s="39" t="n">
         <v>20</v>
       </c>
@@ -1589,15 +1589,15 @@
       <c r="P4" s="52" t="n"/>
       <c r="Q4" s="52" t="n"/>
       <c r="R4" s="35" t="n"/>
-      <c r="S4" s="36" t="n"/>
-      <c r="T4" s="53" t="n"/>
+      <c r="S4" s="36" t="n">
+        <v>12.32</v>
+      </c>
+      <c r="T4" s="53" t="inlineStr"/>
       <c r="U4" s="54" t="n">
         <v>262.98</v>
       </c>
-      <c r="V4" s="38" t="n">
-        <v>12.32</v>
-      </c>
-      <c r="W4" s="55" t="inlineStr"/>
+      <c r="V4" s="38" t="n"/>
+      <c r="W4" s="55" t="n"/>
       <c r="X4" s="56" t="n"/>
       <c r="Y4" s="57" t="n">
         <v>388.03</v>
@@ -1684,15 +1684,15 @@
       <c r="P5" s="33" t="n"/>
       <c r="Q5" s="33" t="n"/>
       <c r="R5" s="35" t="n"/>
-      <c r="S5" s="36" t="n"/>
-      <c r="T5" s="36" t="n"/>
+      <c r="S5" s="36" t="n">
+        <v>17.84</v>
+      </c>
+      <c r="T5" s="36" t="inlineStr"/>
       <c r="U5" s="54" t="n">
         <v>119.55</v>
       </c>
-      <c r="V5" s="38" t="n">
-        <v>17.84</v>
-      </c>
-      <c r="W5" s="38" t="inlineStr"/>
+      <c r="V5" s="38" t="n"/>
+      <c r="W5" s="38" t="n"/>
       <c r="X5" s="63" t="n">
         <v>122.81</v>
       </c>
@@ -1782,15 +1782,15 @@
       <c r="P6" s="11" t="n"/>
       <c r="Q6" s="11" t="n"/>
       <c r="R6" s="12" t="n"/>
-      <c r="S6" s="36" t="n"/>
-      <c r="T6" s="22" t="n"/>
+      <c r="S6" s="36" t="n">
+        <v>38.22</v>
+      </c>
+      <c r="T6" s="22" t="inlineStr"/>
       <c r="U6" s="54" t="n">
         <v>103.93</v>
       </c>
-      <c r="V6" s="38" t="n">
-        <v>38.22</v>
-      </c>
-      <c r="W6" s="67" t="inlineStr"/>
+      <c r="V6" s="38" t="n"/>
+      <c r="W6" s="67" t="n"/>
       <c r="X6" s="63" t="n">
         <v>115.33</v>
       </c>
@@ -1880,15 +1880,15 @@
       <c r="P7" s="78" t="n"/>
       <c r="Q7" s="78" t="n"/>
       <c r="R7" s="78" t="n"/>
-      <c r="S7" s="36" t="n"/>
-      <c r="T7" s="79" t="n"/>
+      <c r="S7" s="36" t="n">
+        <v>35.36</v>
+      </c>
+      <c r="T7" s="79" t="inlineStr"/>
       <c r="U7" s="80" t="n">
         <v>104.4</v>
       </c>
-      <c r="V7" s="38" t="n">
-        <v>35.36</v>
-      </c>
-      <c r="W7" s="81" t="inlineStr"/>
+      <c r="V7" s="38" t="n"/>
+      <c r="W7" s="81" t="n"/>
       <c r="X7" s="82" t="n">
         <v>63.74</v>
       </c>
@@ -2051,15 +2051,15 @@
       <c r="P9" s="11" t="n"/>
       <c r="Q9" s="11" t="n"/>
       <c r="R9" s="12" t="n"/>
-      <c r="S9" s="36" t="n"/>
-      <c r="T9" s="22" t="n"/>
+      <c r="S9" s="36" t="n">
+        <v>8.49</v>
+      </c>
+      <c r="T9" s="22" t="inlineStr"/>
       <c r="U9" s="54" t="n">
         <v>132.97</v>
       </c>
-      <c r="V9" s="38" t="n">
-        <v>8.49</v>
-      </c>
-      <c r="W9" s="67" t="inlineStr"/>
+      <c r="V9" s="38" t="n"/>
+      <c r="W9" s="67" t="n"/>
       <c r="X9" s="63" t="n">
         <v>315.87</v>
       </c>
@@ -2308,15 +2308,15 @@
       <c r="P12" s="11" t="n"/>
       <c r="Q12" s="11" t="n"/>
       <c r="R12" s="12" t="n"/>
-      <c r="S12" s="36" t="n"/>
-      <c r="T12" s="22" t="n"/>
+      <c r="S12" s="36" t="n">
+        <v>0</v>
+      </c>
+      <c r="T12" s="22" t="inlineStr"/>
       <c r="U12" s="54" t="n">
         <v>170.88</v>
       </c>
-      <c r="V12" s="38" t="n">
-        <v>0</v>
-      </c>
-      <c r="W12" s="67" t="inlineStr"/>
+      <c r="V12" s="38" t="n"/>
+      <c r="W12" s="67" t="n"/>
       <c r="X12" s="63" t="n"/>
       <c r="Y12" s="68" t="n"/>
       <c r="Z12" s="13" t="n"/>
@@ -2481,13 +2481,13 @@
       <c r="P14" s="11" t="n"/>
       <c r="Q14" s="11" t="n"/>
       <c r="R14" s="12" t="n"/>
-      <c r="S14" s="36" t="n"/>
-      <c r="T14" s="22" t="n"/>
-      <c r="U14" s="37" t="n"/>
-      <c r="V14" s="38" t="n">
+      <c r="S14" s="36" t="n">
         <v>26.84</v>
       </c>
-      <c r="W14" s="67" t="inlineStr"/>
+      <c r="T14" s="22" t="inlineStr"/>
+      <c r="U14" s="37" t="n"/>
+      <c r="V14" s="38" t="n"/>
+      <c r="W14" s="67" t="n"/>
       <c r="X14" s="39" t="n"/>
       <c r="Y14" s="68" t="n"/>
       <c r="Z14" s="13" t="n"/>
@@ -2569,13 +2569,13 @@
       <c r="P15" s="11" t="n"/>
       <c r="Q15" s="11" t="n"/>
       <c r="R15" s="12" t="n"/>
-      <c r="S15" s="36" t="n"/>
-      <c r="T15" s="22" t="n"/>
-      <c r="U15" s="54" t="n"/>
-      <c r="V15" s="38" t="n">
+      <c r="S15" s="36" t="n">
         <v>5.84</v>
       </c>
-      <c r="W15" s="67" t="inlineStr"/>
+      <c r="T15" s="22" t="inlineStr"/>
+      <c r="U15" s="54" t="n"/>
+      <c r="V15" s="38" t="n"/>
+      <c r="W15" s="67" t="n"/>
       <c r="X15" s="63" t="n">
         <v>132.22</v>
       </c>
@@ -2816,15 +2816,15 @@
       <c r="P18" s="11" t="n"/>
       <c r="Q18" s="11" t="n"/>
       <c r="R18" s="12" t="n"/>
-      <c r="S18" s="36" t="n"/>
-      <c r="T18" s="22" t="n"/>
+      <c r="S18" s="36" t="n">
+        <v>19.61</v>
+      </c>
+      <c r="T18" s="22" t="inlineStr"/>
       <c r="U18" s="23" t="n">
         <v>456.4</v>
       </c>
-      <c r="V18" s="38" t="n">
-        <v>19.61</v>
-      </c>
-      <c r="W18" s="67" t="inlineStr"/>
+      <c r="V18" s="38" t="n"/>
+      <c r="W18" s="67" t="n"/>
       <c r="X18" s="116" t="n">
         <v>369.77</v>
       </c>
@@ -2914,15 +2914,15 @@
       <c r="P19" s="11" t="n"/>
       <c r="Q19" s="11" t="n"/>
       <c r="R19" s="12" t="n"/>
-      <c r="S19" s="36" t="n"/>
-      <c r="T19" s="22" t="n"/>
-      <c r="U19" s="23" t="n"/>
-      <c r="V19" s="38" t="n">
+      <c r="S19" s="36" t="n">
         <v>40</v>
       </c>
-      <c r="W19" s="67" t="n">
+      <c r="T19" s="22" t="n">
         <v>6.369999999999997</v>
       </c>
+      <c r="U19" s="23" t="n"/>
+      <c r="V19" s="38" t="n"/>
+      <c r="W19" s="67" t="n"/>
       <c r="X19" s="116" t="n"/>
       <c r="Y19" s="13" t="n"/>
       <c r="Z19" s="13" t="n"/>
@@ -3007,13 +3007,13 @@
       <c r="P20" s="11" t="n"/>
       <c r="Q20" s="11" t="n"/>
       <c r="R20" s="12" t="n"/>
-      <c r="S20" s="36" t="n"/>
-      <c r="T20" s="22" t="n"/>
-      <c r="U20" s="23" t="n"/>
-      <c r="V20" s="38" t="n">
+      <c r="S20" s="36" t="n">
         <v>3.56</v>
       </c>
-      <c r="W20" s="67" t="inlineStr"/>
+      <c r="T20" s="22" t="inlineStr"/>
+      <c r="U20" s="23" t="n"/>
+      <c r="V20" s="38" t="n"/>
+      <c r="W20" s="67" t="n"/>
       <c r="X20" s="116" t="n">
         <v>79.51000000000001</v>
       </c>
@@ -3100,15 +3100,15 @@
       <c r="P21" s="11" t="n"/>
       <c r="Q21" s="11" t="n"/>
       <c r="R21" s="12" t="n"/>
-      <c r="S21" s="36" t="n"/>
-      <c r="T21" s="22" t="n"/>
+      <c r="S21" s="36" t="n">
+        <v>4.95</v>
+      </c>
+      <c r="T21" s="22" t="inlineStr"/>
       <c r="U21" s="23" t="n">
         <v>139.61</v>
       </c>
-      <c r="V21" s="38" t="n">
-        <v>4.95</v>
-      </c>
-      <c r="W21" s="67" t="inlineStr"/>
+      <c r="V21" s="38" t="n"/>
+      <c r="W21" s="67" t="n"/>
       <c r="X21" s="116" t="n">
         <v>140.54</v>
       </c>
@@ -3185,13 +3185,13 @@
       <c r="P22" s="11" t="n"/>
       <c r="Q22" s="11" t="n"/>
       <c r="R22" s="12" t="n"/>
-      <c r="S22" s="36" t="n"/>
-      <c r="T22" s="22" t="n"/>
-      <c r="U22" s="23" t="n"/>
-      <c r="V22" s="38" t="n">
+      <c r="S22" s="36" t="n">
         <v>8.51</v>
       </c>
-      <c r="W22" s="67" t="inlineStr"/>
+      <c r="T22" s="22" t="inlineStr"/>
+      <c r="U22" s="23" t="n"/>
+      <c r="V22" s="38" t="n"/>
+      <c r="W22" s="67" t="n"/>
       <c r="X22" s="116" t="n"/>
       <c r="Y22" s="13" t="n"/>
       <c r="Z22" s="13" t="n"/>
@@ -3276,15 +3276,15 @@
       <c r="P23" s="11" t="n"/>
       <c r="Q23" s="11" t="n"/>
       <c r="R23" s="12" t="n"/>
-      <c r="S23" s="36" t="n"/>
-      <c r="T23" s="22" t="n"/>
+      <c r="S23" s="36" t="n">
+        <v>4.75</v>
+      </c>
+      <c r="T23" s="22" t="inlineStr"/>
       <c r="U23" s="23" t="n">
         <v>3.15</v>
       </c>
-      <c r="V23" s="38" t="n">
-        <v>4.75</v>
-      </c>
-      <c r="W23" s="67" t="inlineStr"/>
+      <c r="V23" s="38" t="n"/>
+      <c r="W23" s="67" t="n"/>
       <c r="X23" s="116" t="n">
         <v>13.23</v>
       </c>
@@ -3369,15 +3369,15 @@
       <c r="P24" s="11" t="n"/>
       <c r="Q24" s="11" t="n"/>
       <c r="R24" s="12" t="n"/>
-      <c r="S24" s="36" t="n"/>
-      <c r="T24" s="22" t="n"/>
+      <c r="S24" s="36" t="n">
+        <v>32.74</v>
+      </c>
+      <c r="T24" s="22" t="inlineStr"/>
       <c r="U24" s="23" t="n">
         <v>924.16</v>
       </c>
-      <c r="V24" s="38" t="n">
-        <v>32.74</v>
-      </c>
-      <c r="W24" s="67" t="inlineStr"/>
+      <c r="V24" s="38" t="n"/>
+      <c r="W24" s="67" t="n"/>
       <c r="X24" s="116" t="n">
         <v>768.84</v>
       </c>
@@ -3467,17 +3467,17 @@
       <c r="P25" s="11" t="n"/>
       <c r="Q25" s="11" t="n"/>
       <c r="R25" s="12" t="n"/>
-      <c r="S25" s="36" t="n"/>
-      <c r="T25" s="22" t="n"/>
+      <c r="S25" s="36" t="n">
+        <v>40</v>
+      </c>
+      <c r="T25" s="22" t="n">
+        <v>3.979999999999997</v>
+      </c>
       <c r="U25" s="23" t="n">
         <v>141.47</v>
       </c>
-      <c r="V25" s="38" t="n">
-        <v>40</v>
-      </c>
-      <c r="W25" s="67" t="n">
-        <v>3.979999999999997</v>
-      </c>
+      <c r="V25" s="38" t="n"/>
+      <c r="W25" s="67" t="n"/>
       <c r="X25" s="116" t="n"/>
       <c r="Y25" s="13" t="n"/>
       <c r="Z25" s="13" t="n"/>
@@ -3727,15 +3727,15 @@
       <c r="P28" s="11" t="n"/>
       <c r="Q28" s="11" t="n"/>
       <c r="R28" s="12" t="n"/>
-      <c r="S28" s="36" t="n"/>
-      <c r="T28" s="22" t="n"/>
+      <c r="S28" s="36" t="n">
+        <v>18.52</v>
+      </c>
+      <c r="T28" s="22" t="inlineStr"/>
       <c r="U28" s="23" t="n">
         <v>82.06</v>
       </c>
-      <c r="V28" s="38" t="n">
-        <v>18.52</v>
-      </c>
-      <c r="W28" s="24" t="inlineStr"/>
+      <c r="V28" s="38" t="n"/>
+      <c r="W28" s="24" t="n"/>
       <c r="X28" s="25" t="n">
         <v>199.51</v>
       </c>
@@ -3820,15 +3820,15 @@
       <c r="P29" s="11" t="n"/>
       <c r="Q29" s="11" t="n"/>
       <c r="R29" s="12" t="n"/>
-      <c r="S29" s="36" t="n"/>
-      <c r="T29" s="22" t="n"/>
+      <c r="S29" s="36" t="n">
+        <v>32.32</v>
+      </c>
+      <c r="T29" s="22" t="inlineStr"/>
       <c r="U29" s="23" t="n">
         <v>285.58</v>
       </c>
-      <c r="V29" s="38" t="n">
-        <v>32.32</v>
-      </c>
-      <c r="W29" s="24" t="inlineStr"/>
+      <c r="V29" s="38" t="n"/>
+      <c r="W29" s="24" t="n"/>
       <c r="X29" s="25" t="n">
         <v>663.9400000000001</v>
       </c>
@@ -3915,15 +3915,15 @@
       <c r="P30" s="11" t="n"/>
       <c r="Q30" s="11" t="n"/>
       <c r="R30" s="12" t="n"/>
-      <c r="S30" s="36" t="n"/>
-      <c r="T30" s="22" t="n"/>
+      <c r="S30" s="36" t="n">
+        <v>39.39</v>
+      </c>
+      <c r="T30" s="22" t="inlineStr"/>
       <c r="U30" s="23" t="n">
         <v>558.9400000000001</v>
       </c>
-      <c r="V30" s="38" t="n">
-        <v>39.39</v>
-      </c>
-      <c r="W30" s="24" t="inlineStr"/>
+      <c r="V30" s="38" t="n"/>
+      <c r="W30" s="24" t="n"/>
       <c r="X30" s="25" t="n">
         <v>638.92</v>
       </c>
@@ -4010,13 +4010,13 @@
       <c r="P31" s="11" t="n"/>
       <c r="Q31" s="11" t="n"/>
       <c r="R31" s="12" t="n"/>
-      <c r="S31" s="36" t="n"/>
-      <c r="T31" s="22" t="n"/>
-      <c r="U31" s="23" t="n"/>
-      <c r="V31" s="38" t="n">
+      <c r="S31" s="36" t="n">
         <v>26.29</v>
       </c>
-      <c r="W31" s="24" t="inlineStr"/>
+      <c r="T31" s="22" t="inlineStr"/>
+      <c r="U31" s="23" t="n"/>
+      <c r="V31" s="38" t="n"/>
+      <c r="W31" s="24" t="n"/>
       <c r="X31" s="25" t="n"/>
       <c r="Y31" s="13" t="n"/>
       <c r="Z31" s="13" t="n"/>
@@ -4659,10 +4659,10 @@
           <t xml:space="preserve">ANAKA  HOST </t>
         </is>
       </c>
-      <c r="V41" t="n">
+      <c r="S41" t="n">
         <v>21.04</v>
       </c>
-      <c r="W41" t="inlineStr"/>
+      <c r="T41" t="inlineStr"/>
     </row>
     <row r="42" ht="15.75" customHeight="1">
       <c r="B42" s="162" t="inlineStr">
@@ -4670,110 +4670,192 @@
           <t>H-Kimberly Host</t>
         </is>
       </c>
-      <c r="V42" t="n">
+      <c r="S42" t="n">
         <v>10.22</v>
       </c>
-      <c r="W42" t="inlineStr"/>
+      <c r="T42" t="inlineStr"/>
     </row>
     <row r="43" ht="15.75" customHeight="1">
       <c r="B43" s="162" t="inlineStr">
-        <is>
-          <t>H-R Host</t>
-        </is>
-      </c>
-      <c r="V43" t="n">
-        <v>0</v>
-      </c>
-      <c r="W43" t="inlineStr"/>
-    </row>
-    <row r="44" ht="15.75" customHeight="1">
-      <c r="B44" s="162" t="inlineStr">
         <is>
           <t>MATTHEW CHEA</t>
         </is>
       </c>
-      <c r="V44" t="n">
+      <c r="S43" t="n">
         <v>21.5</v>
       </c>
-      <c r="W44" t="inlineStr"/>
-    </row>
-    <row r="45" ht="15.75" customHeight="1">
-      <c r="B45" s="162" t="inlineStr">
-        <is>
-          <t>S-Johnny Server</t>
-        </is>
-      </c>
-      <c r="V45" t="n">
-        <v>0</v>
-      </c>
-      <c r="W45" t="inlineStr"/>
-    </row>
-    <row r="46" ht="15.75" customHeight="1">
-      <c r="B46" s="162" t="inlineStr">
+      <c r="T43" t="inlineStr"/>
+    </row>
+    <row r="44" ht="15.75" customHeight="1">
+      <c r="B44" s="162" t="inlineStr">
         <is>
           <t>S-Kimberly Server</t>
         </is>
       </c>
-      <c r="V46" t="n">
+      <c r="S44" t="n">
         <v>8.34</v>
       </c>
-      <c r="W46" t="inlineStr"/>
-    </row>
-    <row r="47" ht="15.75" customHeight="1">
-      <c r="B47" s="162" t="inlineStr">
+      <c r="T44" t="inlineStr"/>
+    </row>
+    <row r="45" ht="15.75" customHeight="1">
+      <c r="B45" s="162" t="inlineStr">
         <is>
           <t>S-Xa  Server</t>
         </is>
       </c>
-      <c r="V47" t="n">
+      <c r="S45" t="n">
         <v>4.01</v>
       </c>
-      <c r="W47" t="inlineStr"/>
-    </row>
-    <row r="48" ht="15.75" customHeight="1">
-      <c r="A48" s="1" t="n"/>
-      <c r="B48" s="126" t="n"/>
-      <c r="C48" s="126" t="n"/>
-      <c r="D48" s="127" t="n"/>
-      <c r="E48" s="34" t="n"/>
-      <c r="F48" s="30" t="n"/>
-      <c r="G48" s="5" t="n"/>
-      <c r="H48" s="30" t="n"/>
-      <c r="I48" s="34" t="n"/>
-      <c r="J48" s="94" t="n"/>
-      <c r="K48" s="94" t="n"/>
-      <c r="L48" s="34">
+      <c r="T45" t="inlineStr"/>
+    </row>
+    <row r="46" ht="15.75" customHeight="1">
+      <c r="A46" s="1" t="n"/>
+      <c r="B46" s="126" t="n"/>
+      <c r="C46" s="126" t="n"/>
+      <c r="D46" s="127" t="n"/>
+      <c r="E46" s="34" t="n"/>
+      <c r="F46" s="30" t="n"/>
+      <c r="G46" s="5" t="n"/>
+      <c r="H46" s="30" t="n"/>
+      <c r="I46" s="34" t="n"/>
+      <c r="J46" s="94" t="n"/>
+      <c r="K46" s="94" t="n"/>
+      <c r="L46" s="34">
         <f>SUM(L3:L29)</f>
         <v/>
       </c>
-      <c r="M48" s="34">
+      <c r="M46" s="34">
         <f>SUM(M3:M35)</f>
         <v/>
       </c>
-      <c r="N48" s="33" t="n"/>
-      <c r="O48" s="33" t="n"/>
-      <c r="P48" s="33" t="n"/>
-      <c r="Q48" s="33" t="n"/>
-      <c r="R48" s="128">
+      <c r="N46" s="33" t="n"/>
+      <c r="O46" s="33" t="n"/>
+      <c r="P46" s="33" t="n"/>
+      <c r="Q46" s="33" t="n"/>
+      <c r="R46" s="128">
         <f>SUM(R3:R5)</f>
         <v/>
       </c>
-      <c r="S48" s="36" t="n"/>
-      <c r="T48" s="36" t="n"/>
-      <c r="U48" s="34">
+      <c r="S46" s="36" t="n"/>
+      <c r="T46" s="36" t="n"/>
+      <c r="U46" s="34">
         <f>SUM(U3:U35)</f>
         <v/>
       </c>
-      <c r="V48" s="38" t="n"/>
-      <c r="W48" s="38" t="n"/>
-      <c r="X48" s="34">
+      <c r="V46" s="38" t="n"/>
+      <c r="W46" s="38" t="n"/>
+      <c r="X46" s="34">
         <f>SUM(X3:X33)</f>
         <v/>
       </c>
-      <c r="Y48" s="34">
+      <c r="Y46" s="34">
         <f>SUM(Y3:Y33)</f>
         <v/>
       </c>
+      <c r="Z46" s="41" t="n"/>
+      <c r="AA46" s="129" t="n"/>
+      <c r="AB46" s="129" t="n"/>
+      <c r="AC46" s="130" t="n"/>
+      <c r="AD46" s="129" t="n"/>
+      <c r="AE46" s="129" t="n"/>
+      <c r="AF46" s="129" t="n"/>
+      <c r="AG46" s="129" t="n"/>
+      <c r="AH46" s="45" t="n"/>
+      <c r="AI46" s="45" t="n"/>
+      <c r="AJ46" s="45" t="n"/>
+      <c r="AK46" s="46" t="n"/>
+      <c r="AL46" s="46" t="n"/>
+      <c r="AM46" s="46" t="n"/>
+      <c r="AN46" s="46" t="n"/>
+      <c r="AO46" s="46" t="n"/>
+      <c r="AP46" s="46" t="n"/>
+      <c r="AQ46" s="46" t="n"/>
+      <c r="AR46" s="46" t="n"/>
+      <c r="AS46" s="46" t="n"/>
+      <c r="AT46" s="46" t="n"/>
+      <c r="AU46" s="46" t="n"/>
+      <c r="AV46" s="46" t="n"/>
+      <c r="AW46" s="46" t="n"/>
+      <c r="AX46" s="46" t="n"/>
+    </row>
+    <row r="47" ht="15.75" customHeight="1">
+      <c r="A47" s="131" t="n"/>
+      <c r="B47" s="45" t="n"/>
+      <c r="C47" s="45" t="n"/>
+      <c r="D47" s="132" t="n"/>
+      <c r="E47" s="30" t="n"/>
+      <c r="F47" s="133" t="n"/>
+      <c r="G47" s="133" t="n"/>
+      <c r="H47" s="133" t="n"/>
+      <c r="I47" s="134" t="n"/>
+      <c r="J47" s="33" t="n"/>
+      <c r="K47" s="33" t="n"/>
+      <c r="L47" s="33" t="n"/>
+      <c r="M47" s="134" t="n"/>
+      <c r="N47" s="135" t="n"/>
+      <c r="O47" s="135" t="n"/>
+      <c r="P47" s="135" t="n"/>
+      <c r="Q47" s="135" t="n"/>
+      <c r="R47" s="135" t="n"/>
+      <c r="S47" s="136" t="n"/>
+      <c r="T47" s="136" t="n"/>
+      <c r="U47" s="130" t="n"/>
+      <c r="V47" s="136" t="n"/>
+      <c r="W47" s="136" t="n"/>
+      <c r="X47" s="130" t="n"/>
+      <c r="Y47" s="41" t="n"/>
+      <c r="Z47" s="41" t="n"/>
+      <c r="AA47" s="129" t="n"/>
+      <c r="AB47" s="129" t="n"/>
+      <c r="AC47" s="130" t="n"/>
+      <c r="AD47" s="129" t="n"/>
+      <c r="AE47" s="129" t="n"/>
+      <c r="AF47" s="129" t="n"/>
+      <c r="AG47" s="129" t="n"/>
+      <c r="AH47" s="45" t="n"/>
+      <c r="AI47" s="45" t="n"/>
+      <c r="AJ47" s="45" t="n"/>
+      <c r="AK47" s="46" t="n"/>
+      <c r="AL47" s="46" t="n"/>
+      <c r="AM47" s="46" t="n"/>
+      <c r="AN47" s="46" t="n"/>
+      <c r="AO47" s="46" t="n"/>
+      <c r="AP47" s="46" t="n"/>
+      <c r="AQ47" s="46" t="n"/>
+      <c r="AR47" s="46" t="n"/>
+      <c r="AS47" s="46" t="n"/>
+      <c r="AT47" s="46" t="n"/>
+      <c r="AU47" s="46" t="n"/>
+      <c r="AV47" s="46" t="n"/>
+      <c r="AW47" s="46" t="n"/>
+      <c r="AX47" s="46" t="n"/>
+    </row>
+    <row r="48" ht="15.75" customHeight="1">
+      <c r="A48" s="131" t="n"/>
+      <c r="B48" s="45" t="n"/>
+      <c r="C48" s="45" t="n"/>
+      <c r="D48" s="132" t="n"/>
+      <c r="E48" s="30" t="n"/>
+      <c r="F48" s="133" t="n"/>
+      <c r="G48" s="137" t="n"/>
+      <c r="H48" s="133" t="n"/>
+      <c r="I48" s="134" t="n"/>
+      <c r="J48" s="33" t="n"/>
+      <c r="K48" s="33" t="n"/>
+      <c r="L48" s="33" t="n"/>
+      <c r="M48" s="134" t="n"/>
+      <c r="N48" s="135" t="n"/>
+      <c r="O48" s="135" t="n"/>
+      <c r="P48" s="135" t="n"/>
+      <c r="Q48" s="135" t="n"/>
+      <c r="R48" s="135" t="n"/>
+      <c r="S48" s="36" t="n"/>
+      <c r="T48" s="36" t="n"/>
+      <c r="U48" s="23" t="n"/>
+      <c r="V48" s="38" t="n"/>
+      <c r="W48" s="38" t="n"/>
+      <c r="X48" s="116" t="n"/>
+      <c r="Y48" s="41" t="n"/>
       <c r="Z48" s="41" t="n"/>
       <c r="AA48" s="129" t="n"/>
       <c r="AB48" s="129" t="n"/>
@@ -4807,7 +4889,7 @@
       <c r="D49" s="132" t="n"/>
       <c r="E49" s="30" t="n"/>
       <c r="F49" s="133" t="n"/>
-      <c r="G49" s="133" t="n"/>
+      <c r="G49" s="137" t="n"/>
       <c r="H49" s="133" t="n"/>
       <c r="I49" s="134" t="n"/>
       <c r="J49" s="33" t="n"/>
@@ -4819,12 +4901,12 @@
       <c r="P49" s="135" t="n"/>
       <c r="Q49" s="135" t="n"/>
       <c r="R49" s="135" t="n"/>
-      <c r="S49" s="136" t="n"/>
-      <c r="T49" s="136" t="n"/>
-      <c r="U49" s="130" t="n"/>
-      <c r="V49" s="136" t="n"/>
-      <c r="W49" s="136" t="n"/>
-      <c r="X49" s="130" t="n"/>
+      <c r="S49" s="36" t="n"/>
+      <c r="T49" s="36" t="n"/>
+      <c r="U49" s="23" t="n"/>
+      <c r="V49" s="38" t="n"/>
+      <c r="W49" s="38" t="n"/>
+      <c r="X49" s="116" t="n"/>
       <c r="Y49" s="41" t="n"/>
       <c r="Z49" s="41" t="n"/>
       <c r="AA49" s="129" t="n"/>
@@ -4837,20 +4919,20 @@
       <c r="AH49" s="45" t="n"/>
       <c r="AI49" s="45" t="n"/>
       <c r="AJ49" s="45" t="n"/>
-      <c r="AK49" s="46" t="n"/>
-      <c r="AL49" s="46" t="n"/>
-      <c r="AM49" s="46" t="n"/>
-      <c r="AN49" s="46" t="n"/>
-      <c r="AO49" s="46" t="n"/>
-      <c r="AP49" s="46" t="n"/>
-      <c r="AQ49" s="46" t="n"/>
-      <c r="AR49" s="46" t="n"/>
-      <c r="AS49" s="46" t="n"/>
-      <c r="AT49" s="46" t="n"/>
-      <c r="AU49" s="46" t="n"/>
-      <c r="AV49" s="46" t="n"/>
-      <c r="AW49" s="46" t="n"/>
-      <c r="AX49" s="46" t="n"/>
+      <c r="AK49" s="138" t="n"/>
+      <c r="AL49" s="138" t="n"/>
+      <c r="AM49" s="138" t="n"/>
+      <c r="AN49" s="138" t="n"/>
+      <c r="AO49" s="138" t="n"/>
+      <c r="AP49" s="138" t="n"/>
+      <c r="AQ49" s="138" t="n"/>
+      <c r="AR49" s="138" t="n"/>
+      <c r="AS49" s="138" t="n"/>
+      <c r="AT49" s="138" t="n"/>
+      <c r="AU49" s="138" t="n"/>
+      <c r="AV49" s="138" t="n"/>
+      <c r="AW49" s="138" t="n"/>
+      <c r="AX49" s="138" t="n"/>
     </row>
     <row r="50" ht="15.75" customHeight="1">
       <c r="A50" s="131" t="n"/>
@@ -4889,20 +4971,20 @@
       <c r="AH50" s="45" t="n"/>
       <c r="AI50" s="45" t="n"/>
       <c r="AJ50" s="45" t="n"/>
-      <c r="AK50" s="46" t="n"/>
-      <c r="AL50" s="46" t="n"/>
-      <c r="AM50" s="46" t="n"/>
-      <c r="AN50" s="46" t="n"/>
-      <c r="AO50" s="46" t="n"/>
-      <c r="AP50" s="46" t="n"/>
-      <c r="AQ50" s="46" t="n"/>
-      <c r="AR50" s="46" t="n"/>
-      <c r="AS50" s="46" t="n"/>
-      <c r="AT50" s="46" t="n"/>
-      <c r="AU50" s="46" t="n"/>
-      <c r="AV50" s="46" t="n"/>
-      <c r="AW50" s="46" t="n"/>
-      <c r="AX50" s="46" t="n"/>
+      <c r="AK50" s="138" t="n"/>
+      <c r="AL50" s="138" t="n"/>
+      <c r="AM50" s="138" t="n"/>
+      <c r="AN50" s="138" t="n"/>
+      <c r="AO50" s="138" t="n"/>
+      <c r="AP50" s="138" t="n"/>
+      <c r="AQ50" s="138" t="n"/>
+      <c r="AR50" s="138" t="n"/>
+      <c r="AS50" s="138" t="n"/>
+      <c r="AT50" s="138" t="n"/>
+      <c r="AU50" s="138" t="n"/>
+      <c r="AV50" s="138" t="n"/>
+      <c r="AW50" s="138" t="n"/>
+      <c r="AX50" s="138" t="n"/>
     </row>
     <row r="51" ht="15.75" customHeight="1">
       <c r="A51" s="131" t="n"/>
@@ -7661,9 +7743,9 @@
       <c r="AX103" s="138" t="n"/>
     </row>
     <row r="104" ht="13" customHeight="1">
-      <c r="A104" s="131" t="n"/>
-      <c r="B104" s="45" t="n"/>
-      <c r="C104" s="45" t="n"/>
+      <c r="A104" s="139" t="n"/>
+      <c r="B104" s="126" t="n"/>
+      <c r="C104" s="126" t="n"/>
       <c r="D104" s="132" t="n"/>
       <c r="E104" s="30" t="n"/>
       <c r="F104" s="133" t="n"/>
@@ -7713,9 +7795,9 @@
       <c r="AX104" s="138" t="n"/>
     </row>
     <row r="105" ht="13" customHeight="1">
-      <c r="A105" s="131" t="n"/>
-      <c r="B105" s="45" t="n"/>
-      <c r="C105" s="45" t="n"/>
+      <c r="A105" s="139" t="n"/>
+      <c r="B105" s="126" t="n"/>
+      <c r="C105" s="126" t="n"/>
       <c r="D105" s="132" t="n"/>
       <c r="E105" s="30" t="n"/>
       <c r="F105" s="133" t="n"/>
@@ -9689,7 +9771,7 @@
       <c r="AX142" s="138" t="n"/>
     </row>
     <row r="143" ht="13" customHeight="1">
-      <c r="A143" s="139" t="n"/>
+      <c r="A143" s="140" t="n"/>
       <c r="B143" s="126" t="n"/>
       <c r="C143" s="126" t="n"/>
       <c r="D143" s="132" t="n"/>
@@ -9741,7 +9823,7 @@
       <c r="AX143" s="138" t="n"/>
     </row>
     <row r="144" ht="13" customHeight="1">
-      <c r="A144" s="139" t="n"/>
+      <c r="A144" s="140" t="n"/>
       <c r="B144" s="126" t="n"/>
       <c r="C144" s="126" t="n"/>
       <c r="D144" s="132" t="n"/>
@@ -54355,110 +54437,6 @@
       <c r="AV1001" s="138" t="n"/>
       <c r="AW1001" s="138" t="n"/>
       <c r="AX1001" s="138" t="n"/>
-    </row>
-    <row r="1002">
-      <c r="A1002" s="140" t="n"/>
-      <c r="B1002" s="126" t="n"/>
-      <c r="C1002" s="126" t="n"/>
-      <c r="D1002" s="132" t="n"/>
-      <c r="E1002" s="30" t="n"/>
-      <c r="F1002" s="133" t="n"/>
-      <c r="G1002" s="137" t="n"/>
-      <c r="H1002" s="133" t="n"/>
-      <c r="I1002" s="134" t="n"/>
-      <c r="J1002" s="33" t="n"/>
-      <c r="K1002" s="33" t="n"/>
-      <c r="L1002" s="33" t="n"/>
-      <c r="M1002" s="134" t="n"/>
-      <c r="N1002" s="135" t="n"/>
-      <c r="O1002" s="135" t="n"/>
-      <c r="P1002" s="135" t="n"/>
-      <c r="Q1002" s="135" t="n"/>
-      <c r="R1002" s="135" t="n"/>
-      <c r="S1002" s="36" t="n"/>
-      <c r="T1002" s="36" t="n"/>
-      <c r="U1002" s="23" t="n"/>
-      <c r="V1002" s="38" t="n"/>
-      <c r="W1002" s="38" t="n"/>
-      <c r="X1002" s="116" t="n"/>
-      <c r="Y1002" s="41" t="n"/>
-      <c r="Z1002" s="41" t="n"/>
-      <c r="AA1002" s="129" t="n"/>
-      <c r="AB1002" s="129" t="n"/>
-      <c r="AC1002" s="130" t="n"/>
-      <c r="AD1002" s="129" t="n"/>
-      <c r="AE1002" s="129" t="n"/>
-      <c r="AF1002" s="129" t="n"/>
-      <c r="AG1002" s="129" t="n"/>
-      <c r="AH1002" s="45" t="n"/>
-      <c r="AI1002" s="45" t="n"/>
-      <c r="AJ1002" s="45" t="n"/>
-      <c r="AK1002" s="138" t="n"/>
-      <c r="AL1002" s="138" t="n"/>
-      <c r="AM1002" s="138" t="n"/>
-      <c r="AN1002" s="138" t="n"/>
-      <c r="AO1002" s="138" t="n"/>
-      <c r="AP1002" s="138" t="n"/>
-      <c r="AQ1002" s="138" t="n"/>
-      <c r="AR1002" s="138" t="n"/>
-      <c r="AS1002" s="138" t="n"/>
-      <c r="AT1002" s="138" t="n"/>
-      <c r="AU1002" s="138" t="n"/>
-      <c r="AV1002" s="138" t="n"/>
-      <c r="AW1002" s="138" t="n"/>
-      <c r="AX1002" s="138" t="n"/>
-    </row>
-    <row r="1003">
-      <c r="A1003" s="140" t="n"/>
-      <c r="B1003" s="126" t="n"/>
-      <c r="C1003" s="126" t="n"/>
-      <c r="D1003" s="132" t="n"/>
-      <c r="E1003" s="30" t="n"/>
-      <c r="F1003" s="133" t="n"/>
-      <c r="G1003" s="137" t="n"/>
-      <c r="H1003" s="133" t="n"/>
-      <c r="I1003" s="134" t="n"/>
-      <c r="J1003" s="33" t="n"/>
-      <c r="K1003" s="33" t="n"/>
-      <c r="L1003" s="33" t="n"/>
-      <c r="M1003" s="134" t="n"/>
-      <c r="N1003" s="135" t="n"/>
-      <c r="O1003" s="135" t="n"/>
-      <c r="P1003" s="135" t="n"/>
-      <c r="Q1003" s="135" t="n"/>
-      <c r="R1003" s="135" t="n"/>
-      <c r="S1003" s="36" t="n"/>
-      <c r="T1003" s="36" t="n"/>
-      <c r="U1003" s="23" t="n"/>
-      <c r="V1003" s="38" t="n"/>
-      <c r="W1003" s="38" t="n"/>
-      <c r="X1003" s="116" t="n"/>
-      <c r="Y1003" s="41" t="n"/>
-      <c r="Z1003" s="41" t="n"/>
-      <c r="AA1003" s="129" t="n"/>
-      <c r="AB1003" s="129" t="n"/>
-      <c r="AC1003" s="130" t="n"/>
-      <c r="AD1003" s="129" t="n"/>
-      <c r="AE1003" s="129" t="n"/>
-      <c r="AF1003" s="129" t="n"/>
-      <c r="AG1003" s="129" t="n"/>
-      <c r="AH1003" s="45" t="n"/>
-      <c r="AI1003" s="45" t="n"/>
-      <c r="AJ1003" s="45" t="n"/>
-      <c r="AK1003" s="138" t="n"/>
-      <c r="AL1003" s="138" t="n"/>
-      <c r="AM1003" s="138" t="n"/>
-      <c r="AN1003" s="138" t="n"/>
-      <c r="AO1003" s="138" t="n"/>
-      <c r="AP1003" s="138" t="n"/>
-      <c r="AQ1003" s="138" t="n"/>
-      <c r="AR1003" s="138" t="n"/>
-      <c r="AS1003" s="138" t="n"/>
-      <c r="AT1003" s="138" t="n"/>
-      <c r="AU1003" s="138" t="n"/>
-      <c r="AV1003" s="138" t="n"/>
-      <c r="AW1003" s="138" t="n"/>
-      <c r="AX1003" s="138" t="n"/>
     </row>
   </sheetData>
   <autoFilter ref="A2:AG41"/>

</xml_diff>